<commit_message>
Added args TrueString & FalseString to CSVWrite
</commit_message>
<xml_diff>
--- a/workbooks/VBA-CSV-Intellisense.xlsx
+++ b/workbooks/VBA-CSV-Intellisense.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VBA-CSV\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{37BE1114-74FC-4336-BC55-39612EC6D0FD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1036A45-53CE-420F-8911-79E38E2FD6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38498" yWindow="-98" windowWidth="38596" windowHeight="21075" xr2:uid="{DD789D6E-9D66-44FC-984D-A313F056A780}"/>
+    <workbookView xWindow="48503" yWindow="-98" windowWidth="38595" windowHeight="21075" xr2:uid="{CEF2F2E7-CDB7-47C7-BF03-DDC7B4A4CE3D}"/>
   </bookViews>
   <sheets>
     <sheet name="_Intellisense_" sheetId="1" r:id="rId1"/>
@@ -27,6 +27,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="60">
   <si>
     <t>FunctionInfo</t>
   </si>
@@ -202,6 +204,18 @@
   </si>
   <si>
     <t>Controls the line endings of the file written. Enter `Windows` (the default), `Unix` or `Mac`. Also supports the line-ending characters themselves (ascii 13 + ascii 10, ascii 10, ascii 13) or the strings `CRLF`, `LF` or `CR`.</t>
+  </si>
+  <si>
+    <t>TrueString</t>
+  </si>
+  <si>
+    <t>How the Boolean value True is to be represented in the file. Optional, defaulting to "True".</t>
+  </si>
+  <si>
+    <t>FalseString</t>
+  </si>
+  <si>
+    <t>How the Boolean value False is to be represented in the file. Optional, defaulting to "False".</t>
   </si>
 </sst>
 </file>
@@ -558,7 +572,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D91E699-F009-4D30-BC83-58F671F9DAE7}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3D158D-331C-47A0-8D5D-4FB1A896CEA6}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AO3"/>
   <sheetViews>
@@ -586,9 +600,9 @@
     <col min="18" max="18" width="13.73046875" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="40.46484375" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="38.265625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="38.86328125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="39.53125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="9.265625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="39.9296875" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="8.73046875" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="40.19921875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="7.73046875" bestFit="1" customWidth="1"/>
@@ -835,10 +849,18 @@
       <c r="S3" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="T3" s="1"/>
-      <c r="U3" s="1"/>
-      <c r="V3" s="1"/>
-      <c r="W3" s="1"/>
+      <c r="T3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>59</v>
+      </c>
       <c r="X3" s="1"/>
       <c r="Y3" s="1"/>
       <c r="Z3" s="1"/>

</xml_diff>

<commit_message>
Changes to code that creates the intellisense workbook.
</commit_message>
<xml_diff>
--- a/workbooks/VBA-CSV-Intellisense.xlsx
+++ b/workbooks/VBA-CSV-Intellisense.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VBA-CSV\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F1036A45-53CE-420F-8911-79E38E2FD6B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{577582F8-64F4-4377-AACC-3F6308DB3512}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48503" yWindow="-98" windowWidth="38595" windowHeight="21075" xr2:uid="{CEF2F2E7-CDB7-47C7-BF03-DDC7B4A4CE3D}"/>
+    <workbookView xWindow="32302" yWindow="-98" windowWidth="38596" windowHeight="21075" xr2:uid="{5345D018-C091-4F72-95AD-342D6161BE31}"/>
   </bookViews>
   <sheets>
     <sheet name="_Intellisense_" sheetId="1" r:id="rId1"/>
@@ -59,13 +59,35 @@
     <t>ConvertTypes</t>
   </si>
   <si>
-    <t>Type conversion: Boolean or string, subset of letters NDBETQ. N = convert Numbers, D = convert Dates, B = Convert Booleans, E = convert Excel errors, T = trim leading &amp; trailing spaces, Q = quoted fields also converted. TRUE = NDB, FALSE = no conversion.</t>
+    <t>Controls whether fields in the file are converted to typed values or remain as strings, and sets the treatment of "quoted fields" and space characters._x000D_
+_x000D_
+ConvertTypes should be a string of zero or more letters from allowed characters `NDBETQ`._x000D_
+_x000D_
+The most commonly useful letters are:_x000D_
+1) `N` number fields are returned as numbers (Doubles)._x000D_
+2) `D` date fields (that respect DateFormat) are returned as Dates._x000D_
+3) `B` fields matching TrueStrings or FalseStrings are returned as Booleans._x000D_
+_x000D_
+ConvertTypes is optional and defaults to the null string for no type conversion. `TRUE` is equivalent to `NDB` and `FALSE` to the null string._x000D_
+_x000D_
+Three further options are available:_x000D_
+4) `E` fields that match Excel errors are converted to error values. There are fourteen of these, including `#N/A`, `#NAME?`, `#VALUE!` and `#DIV/0!`._x000D_
+5) `T` leading and trailing spaces are trimmed from fields. In the case of quoted fields, this will not remove spaces between the quotes._x000D_
+6) `Q` conversion happens for both quoted and unquoted fields; otherwise only unquoted fields are converted._x000D_
+_x000D_
+For most files, correct type conversion can be achieved with ConvertTypes as a string which applies for all columns, but type conversion can also be specified on a per-column basis._x000D_
+_x000D_
+Enter an array (or range) with two columns or two rows, column numbers on the left/top and type conversion (subset of `NDBETQ`) on the right/bottom. Instead of column numbers, you can enter strings matching the contents of the header row, and a column number of zero applies to all columns not otherwise referenced._x000D_
+_x000D_
+For convenience when calling from VBA, you can pass an array of two element arrays such as `Array(Array(0,"N"),Array(3,""),Array("Phone",""))` to convert all numbers in a file into numbers in the return except for those in column 3 and in the column(s) headed "Phone".</t>
   </si>
   <si>
     <t>Delimiter</t>
   </si>
   <si>
-    <t>Delimiter string. Defaults to the first instance of comma, tab, semi-colon, colon or pipe found outside quoted regions within the first 10,000 characters. Enter FALSE to  see the file's contents as would be displayed in a text editor.</t>
+    <t>By default, CSVRead will try to detect a file's delimiter as the first instance of comma, tab, semi-colon, colon or pipe found outside quoted regions in the first 10,000 characters of the file. If it can't auto-detect the delimiter, it will assume comma. If your file includes a different character or string delimiter you should pass that as the Delimiter argument._x000D_
+_x000D_
+Alternatively, enter `FALSE` as the delimiter to treat the file as "not a delimited file". In this case the return will mimic how the file would appear in a text editor such as NotePad. The file will be split into lines at all line breaks (irrespective of double quotes) and each element of the return will be a line of the file.</t>
   </si>
   <si>
     <t>IgnoreRepeated</t>
@@ -95,7 +117,9 @@
     <t>HeaderRowNum</t>
   </si>
   <si>
-    <t>The row in the file containing headers. Optional and defaults to 0. Type conversion is not applied to fields in the header row, though leading and trailing spaces are trimmed.</t>
+    <t>The row in the file containing headers. Type conversion is not applied to fields in the header row, though leading and trailing spaces are trimmed._x000D_
+_x000D_
+This argument is most useful when calling from VBA, with SkipToRow set to one more than HeaderRowNum. In that case the function returns the rows starting from SkipToRow, and the header row is returned via the by-reference argument HeaderRow. Optional and defaults to 0.</t>
   </si>
   <si>
     <t>SkipToRow</t>
@@ -143,25 +167,27 @@
     <t>ShowMissingsAs</t>
   </si>
   <si>
-    <t>Fields which are missing in the file (consecutive delimiters) or match one of the MissingStrings are returned in the array as ShowMissingsAs. Defaults to Empty, but the null string or `#N/A!` error value can be good alternatives.</t>
+    <t>Fields which are missing in the file (consecutive delimiters) or match one of the MissingStrings are returned in the array as ShowMissingsAs. Defaults to Empty, but the null string or `#N/A!` error value can be good alternatives._x000D_
+_x000D_
+If NumRows is greater than the number of rows in the file then the return is "padded" with the value of ShowMissingsAs. Likewise, if NumCols is greater than the number of columns in the file.</t>
   </si>
   <si>
     <t>Encoding</t>
   </si>
   <si>
-    <t>Allowed entries are `ASCII`, `ANSI`, `UTF-8`, or `UTF-16`. For most files this argument can be omitted and CSVRead will detect the file's encoding.</t>
+    <t>Allowed entries are `ASCII`, `ANSI`, `UTF-8`, or `UTF-16`. For most files this argument can be omitted and CSVRead will detect the file's encoding. If auto-detection does not work, then it's possible that the file is encoded `UTF-8` or `UTF-16` but without a byte option mark to identify the encoding. Experiment with Encoding as each of `UTF-8` and `UTF-16`.</t>
   </si>
   <si>
     <t>DecimalSeparator</t>
   </si>
   <si>
-    <t>The character that represents a decimal point. If omitted, then the value from Windows regional settings is used.</t>
+    <t>In many places in the world, floating point number decimals are separated with a comma instead of a period (3,14 vs. 3.14). CSVRead can correctly parse these numbers by passing in the DecimalSeparator as a comma, in which case comma ceases to be a candidate if the parser needs to guess the Delimiter.</t>
   </si>
   <si>
     <t>HeaderRow</t>
   </si>
   <si>
-    <t>For use from VBA only.</t>
+    <t>This by-reference argument is for use from VBA (as opposed to from Excel formulas). It is populated with the contents of the header row, with no type conversion, though leading and trailing spaces are removed.</t>
   </si>
   <si>
     <t>CSVWrite</t>
@@ -182,7 +208,7 @@
     <t>QuoteAllStrings</t>
   </si>
   <si>
-    <t>If TRUE (the default) then all strings in Data are quoted before being written to file. If FALSE only strings containing Delimiter, line feed, carriage return or double quote are quoted. Double quotes are always escaped by another double quote.</t>
+    <t>If `TRUE` (the default) then elements of Data that are strings are quoted before being written to file, other elements (Numbers, Booleans, Errors) are not quoted. If `FALSE` then the only elements of Data that are quoted are strings containing Delimiter, line feed, carriage return or double quote. In all cases, double quotes are escaped by another double quote.</t>
   </si>
   <si>
     <t>A format string that determines how dates, including cells formatted as dates, appear in the file. If omitted, defaults to `yyyy-mm-dd`.</t>
@@ -203,7 +229,7 @@
     <t>EOL</t>
   </si>
   <si>
-    <t>Controls the line endings of the file written. Enter `Windows` (the default), `Unix` or `Mac`. Also supports the line-ending characters themselves (ascii 13 + ascii 10, ascii 10, ascii 13) or the strings `CRLF`, `LF` or `CR`.</t>
+    <t>Controls the line endings of the file written. Enter `Windows` (the default), `Unix` or `Mac`. Also supports the line-ending characters themselves (ascii 13 + ascii 10, ascii 10, ascii 13) or the strings `CRLF`, `LF` or `CR`. The last line of the file is written with a line ending.</t>
   </si>
   <si>
     <t>TrueString</t>
@@ -572,7 +598,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA3D158D-331C-47A0-8D5D-4FB1A896CEA6}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78352FAC-6422-4F43-B71F-54A9424FACA6}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AO3"/>
   <sheetViews>
@@ -586,7 +612,7 @@
     <col min="4" max="4" width="8.1328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="40.265625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="110.796875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.1328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="40.59765625" customWidth="1"/>
     <col min="10" max="10" width="13.265625" bestFit="1" customWidth="1"/>
@@ -614,13 +640,13 @@
     <col min="32" max="32" width="12.06640625" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="40" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="40.53125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="40.59765625" customWidth="1"/>
     <col min="36" max="36" width="7.86328125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="36.86328125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="39.3984375" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="14.796875" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="39" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="38.53125" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="9.86328125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="38.59765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.45">
@@ -670,7 +696,7 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
     </row>
-    <row r="2" spans="1:41" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:41" ht="409.5" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -793,7 +819,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:41" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:41" ht="114" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
Bug fixes (with added tests) to two edge cases.
Version	Date	Time	Author	Comment
163	02-Nov-2022	19:24	Philip Swannell	Help changes
162	02-Nov-2022	19:05	Philip Swannell	CSVWrite was not correctly handling argument QuoteAllStrings when the delimiter was not a comma. CSVRead fix to another edge case re ragged files and ShowMissingsAs.
</commit_message>
<xml_diff>
--- a/workbooks/VBA-CSV-Intellisense.xlsx
+++ b/workbooks/VBA-CSV-Intellisense.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VBA-CSV\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C10DB87-AC75-4D7E-9698-E0A5368E89CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{50704200-CC3B-4215-B3E8-7DE4812A902D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32302" yWindow="-98" windowWidth="38596" windowHeight="21075" xr2:uid="{273599CE-01EC-48C4-A28F-DAB822A8142D}"/>
+    <workbookView xWindow="32302" yWindow="-98" windowWidth="38596" windowHeight="21075" xr2:uid="{DC31DF96-0F91-4080-A406-04483B7E9B5F}"/>
   </bookViews>
   <sheets>
     <sheet name="_Intellisense_" sheetId="1" r:id="rId1"/>
@@ -233,7 +233,7 @@
     <t>EOL</t>
   </si>
   <si>
-    <t>Controls the line endings of the file written. Enter `Windows` (the default), `Unix` or `Mac`. Also supports the line-ending characters themselves (ascii 13 + ascii 10, ascii 10, ascii 13) or the strings `CRLF`, `LF` or `CR`. The last line of the file is written with a line ending.</t>
+    <t>Sets the file's line endings. Enter `Windows`, `Unix` or `Mac`. Also supports the line-ending characters themselves (ascii 13 + ascii 10, ascii 10, ascii 13) or the strings `CRLF`, `LF` or `CR`. The default is `Windows` if FileName is provided, or `Unix` if not. The last line of the file is written with a line ending.</t>
   </si>
   <si>
     <t>TrueString</t>
@@ -602,7 +602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{220C3934-57E2-490D-BEC2-8933A06E6980}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E2363BD3-7CB9-4325-816D-0BF864898D52}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AO3"/>
   <sheetViews>
@@ -628,7 +628,7 @@
     <col min="16" max="16" width="14.73046875" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="40.53125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="13.73046875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.46484375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.53125" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="39.53125" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="9.265625" bestFit="1" customWidth="1"/>

</xml_diff>

<commit_message>
Improved guessing of the delimiter, with additional tests.
Version	Date	Time	Author	Comment
168	03-Nov-2022	18:25	Philip Swannell	Method InferDelimiter could return an incorrect result for UTF-8 and UTF-16 files (because the BOM was being read as part of the file's contents). Fixed this.
167	03-Nov-2022	16:43	Philip Swannell	Improved method InferDelimiter to avoid interpreting the colon inside a date-with-time field as the file delimiter.
</commit_message>
<xml_diff>
--- a/workbooks/VBA-CSV-Intellisense.xlsx
+++ b/workbooks/VBA-CSV-Intellisense.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VBA-CSV\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A46880DC-23EE-43FD-9661-60D4EA8BF26B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A853990-65A5-4019-B94E-D7EBC90DA9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15675" xr2:uid="{8D9DC5E1-1016-4D80-9E2B-82A2DBBBE9B7}"/>
+    <workbookView xWindow="32302" yWindow="-98" windowWidth="38596" windowHeight="21075" xr2:uid="{40C3A3FD-E0FD-4B00-9BD2-4497FBCC6BA9}"/>
   </bookViews>
   <sheets>
     <sheet name="_Intellisense_" sheetId="1" r:id="rId1"/>
@@ -87,7 +87,7 @@
     <t>Delimiter</t>
   </si>
   <si>
-    <t>By default, CSVRead will try to detect a file's delimiter as the first instance of comma, tab, semi-colon, colon or pipe found outside quoted regions in the first 10,000 characters of the file. If it can't auto-detect the delimiter, it will assume comma. If your file includes a different character or string delimiter you should pass that as the Delimiter argument._x000D_
+    <t>By default, CSVRead will try to detect a file's delimiter as the first instance of comma, tab, semi-colon, colon or pipe found in the first 10,000 characters of the file, searching only outside of quoted regions and outside of date-with-time fields (since these contain colons). If it can't auto-detect the delimiter, it will assume comma. If your file includes a different character or string delimiter you should pass that as the Delimiter argument._x000D_
 _x000D_
 Alternatively, enter `FALSE` as the delimiter to treat the file as "not a delimited file". In this case the return will mimic how the file would appear in a text editor such as NotePad. The file will be split into lines at all line breaks (irrespective of double quotes) and each element of the return will be a line of the file.</t>
   </si>
@@ -602,7 +602,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D7D557B6-4098-41FC-B55E-4F490E001395}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54EF88AA-AC65-4E5A-BBF5-9BDC5DF95FDA}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AO3"/>
   <sheetViews>

</xml_diff>

<commit_message>
CharSet is now "windows-1252" for ANSI
</commit_message>
<xml_diff>
--- a/workbooks/VBA-CSV-Intellisense.xlsx
+++ b/workbooks/VBA-CSV-Intellisense.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VBA-CSV\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5A853990-65A5-4019-B94E-D7EBC90DA9AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9290A3AD-F5D0-4F61-AB68-93F447810019}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32302" yWindow="-98" windowWidth="38596" windowHeight="21075" xr2:uid="{40C3A3FD-E0FD-4B00-9BD2-4497FBCC6BA9}"/>
+    <workbookView xWindow="32302" yWindow="-98" windowWidth="38596" windowHeight="21075" xr2:uid="{CCDDC829-BD49-4ACC-84F3-59BE87229B13}"/>
   </bookViews>
   <sheets>
     <sheet name="_Intellisense_" sheetId="1" r:id="rId1"/>
@@ -177,7 +177,9 @@
     <t>Encoding</t>
   </si>
   <si>
-    <t>Allowed entries are `ASCII`, `ANSI`, `UTF-8`, or `UTF-16`. For most files this argument can be omitted and CSVRead will detect the file's encoding. If auto-detection does not work, then it's possible that the file is encoded `UTF-8` or `UTF-16` but without a byte option mark to identify the encoding. Experiment with Encoding as each of `UTF-8` and `UTF-16`.</t>
+    <t>Allowed entries are `ASCII`, `ANSI`, `UTF-8`, or `UTF-16`. For most files this argument can be omitted and CSVRead will detect the file's encoding. If auto-detection does not work, then it's possible that the file is encoded `UTF-8` or `UTF-16` but without a byte option mark to identify the encoding. Experiment with Encoding as each of `UTF-8` and `UTF-16`._x000D_
+_x000D_
+`ANSI` is taken to mean `Windows-1252` encoding.</t>
   </si>
   <si>
     <t>DecimalSeparator</t>
@@ -602,7 +604,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54EF88AA-AC65-4E5A-BBF5-9BDC5DF95FDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E65CAAE6-7F86-41D0-A098-77BBB45E756C}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AO3"/>
   <sheetViews>

</xml_diff>

<commit_message>
Work in progress (K option for ConvertTypes)
</commit_message>
<xml_diff>
--- a/workbooks/VBA-CSV-Intellisense.xlsx
+++ b/workbooks/VBA-CSV-Intellisense.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VBA-CSV\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{026F3A85-5A99-497A-B4C1-B6994C14B60A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C2A4791-BF90-4F95-B795-E17266AB9D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{B3B4D9B6-B577-48AC-9CBF-89E2BCB353D6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{22227E74-7BE8-4E61-AFA5-7598355CA0FD}"/>
   </bookViews>
   <sheets>
     <sheet name="_Intellisense_" sheetId="1" r:id="rId1"/>
@@ -63,7 +63,7 @@
   <si>
     <t>Controls whether fields in the file are converted to typed values or remain as strings, and sets the treatment of "quoted fields" and space characters._x000D_
 _x000D_
-ConvertTypes should be a string of zero or more letters from allowed characters `NDBETQ`._x000D_
+ConvertTypes should be a string of zero or more letters from allowed characters `NDBETQK`._x000D_
 _x000D_
 The most commonly useful letters are:_x000D_
 1) `N` number fields are returned as numbers (Doubles)._x000D_
@@ -72,14 +72,15 @@
 _x000D_
 ConvertTypes is optional and defaults to the null string for no type conversion. `TRUE` is equivalent to `NDB` and `FALSE` to the null string._x000D_
 _x000D_
-Three further options are available:_x000D_
+Four further options are available:_x000D_
 4) `E` fields that match Excel errors are converted to error values. There are fourteen of these, including `#N/A`, `#NAME?`, `#VALUE!` and `#DIV/0!`._x000D_
 5) `T` leading and trailing spaces are trimmed from fields. In the case of quoted fields, this will not remove spaces between the quotes._x000D_
 6) `Q` conversion happens for both quoted and unquoted fields; otherwise only unquoted fields are converted._x000D_
+7) `K` quoted fields are returned with their quotes kept in place._x000D_
 _x000D_
 For most files, correct type conversion can be achieved with ConvertTypes as a string which applies for all columns, but type conversion can also be specified on a per-column basis._x000D_
 _x000D_
-Enter an array (or range) with two columns or two rows, column numbers on the left/top and type conversion (subset of `NDBETQ`) on the right/bottom. Instead of column numbers, you can enter strings matching the contents of the header row, and a column number of zero applies to all columns not otherwise referenced._x000D_
+Enter an array (or range) with two columns or two rows, column numbers on the left/top and type conversion (subset of `NDBETQK`) on the right/bottom. Instead of column numbers, you can enter strings matching the contents of the header row, and a column number of zero applies to all columns not otherwise referenced._x000D_
 _x000D_
 For convenience when calling from VBA, you can pass an array of two element arrays such as `Array(Array(0,"N"),Array(3,""),Array("Phone",""))` to convert all numbers in a file into numbers in the return except for those in column 3 and in the column(s) headed "Phone".</t>
   </si>
@@ -604,57 +605,57 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00CE9C91-99DE-4514-82D6-3CCC1427AA7F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA417DCB-B3CF-4B49-9BCA-A2C981C06A8A}">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AO3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.36328125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="40.54296875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.6328125" customWidth="1"/>
-    <col min="4" max="4" width="8.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.1796875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1796875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="116.90625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="40.36328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="40.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="39.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="39.81640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="39.90625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="14.6328125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="40.6328125" customWidth="1"/>
-    <col min="20" max="20" width="9.90625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="39.90625" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="9.7265625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="39.90625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="9.26953125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="39.7265625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="8.26953125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="39.08984375" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.1796875" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="39.26953125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="39.36328125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="12.6328125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="39.6328125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="14.54296875" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="39.81640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="8.36328125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="39.54296875" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="15.7265625" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="40.453125" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="39.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="40.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="134" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="40.7109375" customWidth="1"/>
+    <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="40.7109375" customWidth="1"/>
+    <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="40.7109375" customWidth="1"/>
+    <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="37.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="40.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="40.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="11" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="40.7109375" customWidth="1"/>
+    <col min="30" max="30" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="40.7109375" customWidth="1"/>
+    <col min="32" max="32" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="40.7109375" customWidth="1"/>
+    <col min="34" max="34" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="9" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="40.5703125" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="40.7109375" customWidth="1"/>
+    <col min="40" max="40" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="40.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -701,7 +702,7 @@
       <c r="AN1" s="1"/>
       <c r="AO1" s="1"/>
     </row>
-    <row r="2" spans="1:41" ht="409.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:41" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -824,7 +825,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:41" ht="130.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:41" ht="150" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>

<commit_message>
CSVWrite now supports UTF-8NOBOM and UTF-16NOBOM
</commit_message>
<xml_diff>
--- a/workbooks/VBA-CSV-Intellisense.xlsx
+++ b/workbooks/VBA-CSV-Intellisense.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\VBA-CSV\workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6C2A4791-BF90-4F95-B795-E17266AB9D12}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BBA47013-8D24-45CE-89D2-81963AB7FD55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{22227E74-7BE8-4E61-AFA5-7598355CA0FD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{FEBD9EEE-D94F-4378-BC4E-046EF4E9E8DF}"/>
   </bookViews>
   <sheets>
     <sheet name="_Intellisense_" sheetId="1" r:id="rId1"/>
@@ -178,7 +178,7 @@
     <t>Encoding</t>
   </si>
   <si>
-    <t>Allowed entries are `ASCII`, `ANSI`, `UTF-8`, or `UTF-16`. For most files this argument can be omitted and CSVRead will detect the file's encoding. If auto-detection does not work, then it's possible that the file is encoded `UTF-8` or `UTF-16` but without a byte option mark to identify the encoding. Experiment with Encoding as each of `UTF-8` and `UTF-16`._x000D_
+    <t>Allowed entries are `ASCII`, `ANSI`, `UTF-8`, or `UTF-16`. For most files this argument can be omitted and CSVRead will detect the file's encoding. If auto-detection does not work, then it's possible that the file is encoded `UTF-8` or `UTF-16` but without a byte order mark to identify the encoding. Experiment with Encoding as each of `UTF-8` and `UTF-16`._x000D_
 _x000D_
 `ANSI` is taken to mean `Windows-1252` encoding.</t>
   </si>
@@ -215,7 +215,7 @@
     <t>QuoteAllStrings</t>
   </si>
   <si>
-    <t>If `TRUE` (the default) then elements of Data that are strings are quoted before being written to file, other elements (Numbers, Booleans, Errors) are not quoted. If `FALSE` then the only elements of Data that are quoted are strings containing Delimiter, line feed, carriage return or double quote. In all cases, double quotes are escaped by another double quote.</t>
+    <t>If `TRUE` (the default) then elements of Data that are strings are quoted before being written to file, other elements (Numbers, Booleans, Errors) are not quoted. If `FALSE` then the only elements of Data that are quoted are strings containing Delimiter, line feed, carriage return or double quote. In both cases, double quotes are escaped by another double quote. If "Raw" then no strings are quoted. Use this option with care, the file written may not be in valid CSV format.</t>
   </si>
   <si>
     <t>A format string that determines how dates, including cells formatted as dates, appear in the file. If omitted, defaults to `yyyy-mm-dd`.</t>
@@ -230,7 +230,7 @@
     <t>The delimiter string, if omitted defaults to a comma. Delimiter may have more than one character.</t>
   </si>
   <si>
-    <t>Allowed entries are `ANSI` (the default), `UTF-8` and `UTF-16`. An error will result if this argument is `ANSI` but Data contains characters that cannot be written to an ANSI file. `UTF-8` and `UTF-16` files are written with a byte option mark.</t>
+    <t>Allowed entries are `ANSI` (the default), `UTF-8`, `UTF-16`, `UTF-8NOBOM` and `UTF-16NOBOM`. An error will result if this argument is `ANSI` but Data contains characters with code point above 127.</t>
   </si>
   <si>
     <t>EOL</t>
@@ -605,7 +605,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA417DCB-B3CF-4B49-9BCA-A2C981C06A8A}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71C4B028-0F60-436B-9AFD-C0C1D80E0290}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AO3"/>
   <sheetViews>
@@ -628,7 +628,7 @@
     <col min="14" max="14" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="40.7109375" customWidth="1"/>
     <col min="16" max="16" width="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="40.7109375" customWidth="1"/>
+    <col min="17" max="17" width="40.140625" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="15.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="40.7109375" customWidth="1"/>
     <col min="20" max="20" width="10.7109375" bestFit="1" customWidth="1"/>
@@ -825,7 +825,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:41" ht="150" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:41" ht="180" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>42</v>
       </c>

</xml_diff>